<commit_message>
Adding gate works. Some bugs tho in is_Critical
</commit_message>
<xml_diff>
--- a/Villa_output_TD.xlsx
+++ b/Villa_output_TD.xlsx
@@ -521,10 +521,10 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>4.440892098500626e-14</v>
+        <v>1.4210854715202e-14</v>
       </c>
       <c r="L2" t="n">
-        <v>4.440892098500626e-14</v>
+        <v>1.4210854715202e-14</v>
       </c>
       <c r="M2" t="b">
         <v>0</v>
@@ -569,13 +569,13 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>12.82410147924607</v>
+        <v>18</v>
       </c>
       <c r="K3" t="n">
-        <v>4.440892098500626e-14</v>
+        <v>1.4210854715202e-14</v>
       </c>
       <c r="L3" t="n">
-        <v>12.82410147924611</v>
+        <v>13.44304095596299</v>
       </c>
       <c r="M3" t="b">
         <v>0</v>
@@ -617,16 +617,16 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>12.82410147924607</v>
+        <v>18</v>
       </c>
       <c r="J4" t="n">
-        <v>19.84201837430126</v>
+        <v>27</v>
       </c>
       <c r="K4" t="n">
-        <v>12.82410147924611</v>
+        <v>15.08191039316677</v>
       </c>
       <c r="L4" t="n">
-        <v>19.8420183743013</v>
+        <v>19.52580542088384</v>
       </c>
       <c r="M4" t="b">
         <v>0</v>
@@ -668,16 +668,16 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>12.82410147924607</v>
+        <v>18</v>
       </c>
       <c r="J5" t="n">
-        <v>18.68091729304283</v>
+        <v>27</v>
       </c>
       <c r="K5" t="n">
-        <v>13.98520256050455</v>
+        <v>13.44304095596299</v>
       </c>
       <c r="L5" t="n">
-        <v>19.8420183743013</v>
+        <v>19.52580542088384</v>
       </c>
       <c r="M5" t="b">
         <v>0</v>
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>12.82410147924607</v>
+        <v>18</v>
       </c>
       <c r="J6" t="n">
-        <v>16.10424952270873</v>
+        <v>24</v>
       </c>
       <c r="K6" t="n">
-        <v>16.56187033083864</v>
+        <v>15.63700351079632</v>
       </c>
       <c r="L6" t="n">
-        <v>19.8420183743013</v>
+        <v>19.52580542088384</v>
       </c>
       <c r="M6" t="b">
         <v>0</v>
@@ -770,16 +770,16 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>19.84201837430126</v>
+        <v>27</v>
       </c>
       <c r="J7" t="n">
-        <v>23.86205329007482</v>
+        <v>33</v>
       </c>
       <c r="K7" t="n">
-        <v>19.8420183743013</v>
+        <v>19.52580542088384</v>
       </c>
       <c r="L7" t="n">
-        <v>23.86205329007486</v>
+        <v>22.32561713860608</v>
       </c>
       <c r="M7" t="b">
         <v>0</v>
@@ -821,16 +821,16 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>23.86205329007482</v>
+        <v>33</v>
       </c>
       <c r="J8" t="n">
-        <v>28.29023498254501</v>
+        <v>42</v>
       </c>
       <c r="K8" t="n">
-        <v>28.81657189215077</v>
+        <v>25.79809015496251</v>
       </c>
       <c r="L8" t="n">
-        <v>33.24475358462095</v>
+        <v>29.41820997946633</v>
       </c>
       <c r="M8" t="b">
         <v>0</v>
@@ -872,16 +872,16 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>23.86205329007482</v>
+        <v>33</v>
       </c>
       <c r="J9" t="n">
-        <v>33.24475358462091</v>
+        <v>45</v>
       </c>
       <c r="K9" t="n">
-        <v>23.86205329007486</v>
+        <v>22.32561713860608</v>
       </c>
       <c r="L9" t="n">
-        <v>33.24475358462095</v>
+        <v>29.41820997946633</v>
       </c>
       <c r="M9" t="b">
         <v>0</v>
@@ -923,16 +923,16 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>23.86205329007482</v>
+        <v>33</v>
       </c>
       <c r="J10" t="n">
-        <v>30.86937916303991</v>
+        <v>42</v>
       </c>
       <c r="K10" t="n">
-        <v>26.23742771165586</v>
+        <v>25.04554671439056</v>
       </c>
       <c r="L10" t="n">
-        <v>33.24475358462095</v>
+        <v>29.41820997946633</v>
       </c>
       <c r="M10" t="b">
         <v>0</v>
@@ -974,16 +974,16 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>33.24475358462091</v>
+        <v>45</v>
       </c>
       <c r="J11" t="n">
-        <v>41.99486281430161</v>
+        <v>57</v>
       </c>
       <c r="K11" t="n">
-        <v>33.24475358462095</v>
+        <v>29.41820997946633</v>
       </c>
       <c r="L11" t="n">
-        <v>41.99486281430165</v>
+        <v>38.72905499747877</v>
       </c>
       <c r="M11" t="b">
         <v>0</v>
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>41.99486281430161</v>
+        <v>57</v>
       </c>
       <c r="J12" t="n">
-        <v>47.5260992710996</v>
+        <v>66</v>
       </c>
       <c r="K12" t="n">
-        <v>41.99486281430165</v>
+        <v>38.72905499747877</v>
       </c>
       <c r="L12" t="n">
-        <v>47.52609927109965</v>
+        <v>43.38136781397451</v>
       </c>
       <c r="M12" t="b">
         <v>0</v>
@@ -1076,16 +1076,16 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>41.99486281430161</v>
+        <v>57</v>
       </c>
       <c r="J13" t="n">
-        <v>46.36111430885342</v>
+        <v>63</v>
       </c>
       <c r="K13" t="n">
-        <v>43.15984777654784</v>
+        <v>39.11351783178653</v>
       </c>
       <c r="L13" t="n">
-        <v>47.52609927109965</v>
+        <v>43.38136781397451</v>
       </c>
       <c r="M13" t="b">
         <v>0</v>
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>47.5260992710996</v>
+        <v>66</v>
       </c>
       <c r="J14" t="n">
-        <v>51.82695769156489</v>
+        <v>72</v>
       </c>
       <c r="K14" t="n">
-        <v>47.52609927109965</v>
+        <v>43.38136781397451</v>
       </c>
       <c r="L14" t="n">
-        <v>51.82695769156493</v>
+        <v>46.98092793045322</v>
       </c>
       <c r="M14" t="b">
         <v>0</v>
@@ -1178,16 +1178,16 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>51.82695769156489</v>
+        <v>72</v>
       </c>
       <c r="J15" t="n">
-        <v>66.03694031231127</v>
+        <v>90</v>
       </c>
       <c r="K15" t="n">
-        <v>51.82695769156493</v>
+        <v>46.98092793045322</v>
       </c>
       <c r="L15" t="n">
-        <v>66.03694031231132</v>
+        <v>55.97276790034562</v>
       </c>
       <c r="M15" t="b">
         <v>0</v>
@@ -1229,16 +1229,16 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>66.03694031231127</v>
+        <v>90</v>
       </c>
       <c r="J16" t="n">
-        <v>89.91056754984345</v>
+        <v>120</v>
       </c>
       <c r="K16" t="n">
-        <v>66.03694031231132</v>
+        <v>55.97276790034562</v>
       </c>
       <c r="L16" t="n">
-        <v>89.91056754984348</v>
+        <v>68.04303058184443</v>
       </c>
       <c r="M16" t="b">
         <v>0</v>
@@ -1280,16 +1280,16 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>89.91056754984345</v>
+        <v>120</v>
       </c>
       <c r="J17" t="n">
-        <v>103.5883663992811</v>
+        <v>147</v>
       </c>
       <c r="K17" t="n">
-        <v>89.91056754984348</v>
+        <v>68.04303058184443</v>
       </c>
       <c r="L17" t="n">
-        <v>103.5883663992812</v>
+        <v>85.45746142124123</v>
       </c>
       <c r="M17" t="b">
         <v>0</v>
@@ -1331,16 +1331,16 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>103.5883663992811</v>
+        <v>147</v>
       </c>
       <c r="J18" t="n">
-        <v>127.0277263069675</v>
+        <v>177</v>
       </c>
       <c r="K18" t="n">
-        <v>103.5883663992812</v>
+        <v>97.72318716379047</v>
       </c>
       <c r="L18" t="n">
-        <v>127.0277263069675</v>
+        <v>115.7908874891582</v>
       </c>
       <c r="M18" t="b">
         <v>0</v>
@@ -1382,16 +1382,16 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>103.5883663992811</v>
+        <v>147</v>
       </c>
       <c r="J19" t="n">
-        <v>126.3054686085391</v>
+        <v>192</v>
       </c>
       <c r="K19" t="n">
-        <v>104.3106240977095</v>
+        <v>85.45746142124123</v>
       </c>
       <c r="L19" t="n">
-        <v>127.0277263069675</v>
+        <v>115.7908874891582</v>
       </c>
       <c r="M19" t="b">
         <v>0</v>
@@ -1433,16 +1433,16 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>127.0277263069675</v>
+        <v>192</v>
       </c>
       <c r="J20" t="n">
-        <v>138.3623166265677</v>
+        <v>216</v>
       </c>
       <c r="K20" t="n">
-        <v>127.0277263069675</v>
+        <v>115.7908874891582</v>
       </c>
       <c r="L20" t="n">
-        <v>138.3623166265678</v>
+        <v>126.172413280159</v>
       </c>
       <c r="M20" t="b">
         <v>0</v>
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>138.3623166265677</v>
+        <v>216</v>
       </c>
       <c r="J21" t="n">
-        <v>144.5064826874462</v>
+        <v>225</v>
       </c>
       <c r="K21" t="n">
-        <v>143.6645340532007</v>
+        <v>129.7778544756666</v>
       </c>
       <c r="L21" t="n">
-        <v>149.8087001140792</v>
+        <v>136.1631983179873</v>
       </c>
       <c r="M21" t="b">
         <v>0</v>
@@ -1535,16 +1535,16 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>138.3623166265677</v>
+        <v>216</v>
       </c>
       <c r="J22" t="n">
-        <v>149.8087001140792</v>
+        <v>234</v>
       </c>
       <c r="K22" t="n">
-        <v>138.3623166265678</v>
+        <v>126.172413280159</v>
       </c>
       <c r="L22" t="n">
-        <v>149.8087001140792</v>
+        <v>136.1631983179873</v>
       </c>
       <c r="M22" t="b">
         <v>0</v>
@@ -1586,16 +1586,16 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>138.3623166265677</v>
+        <v>216</v>
       </c>
       <c r="J23" t="n">
-        <v>143.8042739524161</v>
+        <v>225</v>
       </c>
       <c r="K23" t="n">
-        <v>144.3667427882309</v>
+        <v>130.5428691997917</v>
       </c>
       <c r="L23" t="n">
-        <v>149.8087001140792</v>
+        <v>136.1631983179873</v>
       </c>
       <c r="M23" t="b">
         <v>0</v>
@@ -1637,16 +1637,16 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>138.3623166265677</v>
+        <v>216</v>
       </c>
       <c r="J24" t="n">
-        <v>143.1731042542695</v>
+        <v>222</v>
       </c>
       <c r="K24" t="n">
-        <v>144.9979124863775</v>
+        <v>132.8332923367175</v>
       </c>
       <c r="L24" t="n">
-        <v>149.8087001140792</v>
+        <v>136.1631983179873</v>
       </c>
       <c r="M24" t="b">
         <v>0</v>
@@ -1688,16 +1688,16 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>149.8087001140792</v>
+        <v>234</v>
       </c>
       <c r="J25" t="n">
-        <v>155.6244276983062</v>
+        <v>246</v>
       </c>
       <c r="K25" t="n">
-        <v>149.8087001140792</v>
+        <v>136.1631983179873</v>
       </c>
       <c r="L25" t="n">
-        <v>155.6244276983062</v>
+        <v>142.0509972493321</v>
       </c>
       <c r="M25" t="b">
         <v>0</v>
@@ -1739,16 +1739,16 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>155.6244276983062</v>
+        <v>246</v>
       </c>
       <c r="J26" t="n">
-        <v>162.3686382345522</v>
+        <v>258</v>
       </c>
       <c r="K26" t="n">
-        <v>155.6244276983062</v>
+        <v>142.0509972493321</v>
       </c>
       <c r="L26" t="n">
-        <v>162.3686382345522</v>
+        <v>147.7975100160089</v>
       </c>
       <c r="M26" t="b">
         <v>0</v>
@@ -1790,16 +1790,16 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>155.6244276983062</v>
+        <v>246</v>
       </c>
       <c r="J27" t="n">
-        <v>161.7859787050823</v>
+        <v>255</v>
       </c>
       <c r="K27" t="n">
-        <v>156.2070872277761</v>
+        <v>143.5701975149649</v>
       </c>
       <c r="L27" t="n">
-        <v>162.3686382345522</v>
+        <v>147.7975100160089</v>
       </c>
       <c r="M27" t="b">
         <v>0</v>
@@ -1841,16 +1841,16 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>155.6244276983062</v>
+        <v>246</v>
       </c>
       <c r="J28" t="n">
-        <v>159.930683377692</v>
+        <v>252</v>
       </c>
       <c r="K28" t="n">
-        <v>158.0623825551664</v>
+        <v>143.2288103544338</v>
       </c>
       <c r="L28" t="n">
-        <v>162.3686382345522</v>
+        <v>147.7975100160089</v>
       </c>
       <c r="M28" t="b">
         <v>0</v>
@@ -1892,16 +1892,16 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>155.6244276983062</v>
+        <v>246</v>
       </c>
       <c r="J29" t="n">
-        <v>160.3909588934673</v>
+        <v>252</v>
       </c>
       <c r="K29" t="n">
-        <v>157.6021070393911</v>
+        <v>143.1905713745582</v>
       </c>
       <c r="L29" t="n">
-        <v>162.3686382345522</v>
+        <v>147.7975100160089</v>
       </c>
       <c r="M29" t="b">
         <v>0</v>
@@ -1943,16 +1943,16 @@
         </is>
       </c>
       <c r="I30" t="n">
-        <v>162.3686382345522</v>
+        <v>258</v>
       </c>
       <c r="J30" t="n">
-        <v>171.4356150430969</v>
+        <v>270</v>
       </c>
       <c r="K30" t="n">
-        <v>162.3686382345522</v>
+        <v>147.7975100160089</v>
       </c>
       <c r="L30" t="n">
-        <v>171.4356150430969</v>
+        <v>154.9364531885381</v>
       </c>
       <c r="M30" t="b">
         <v>0</v>
@@ -1994,16 +1994,16 @@
         </is>
       </c>
       <c r="I31" t="n">
-        <v>171.4356150430969</v>
+        <v>270</v>
       </c>
       <c r="J31" t="n">
-        <v>180.7498642476662</v>
+        <v>282</v>
       </c>
       <c r="K31" t="n">
-        <v>171.4356150430969</v>
+        <v>154.9364531885381</v>
       </c>
       <c r="L31" t="n">
-        <v>180.7498642476663</v>
+        <v>160.1605965196842</v>
       </c>
       <c r="M31" t="b">
         <v>0</v>
@@ -2045,16 +2045,16 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>171.4356150430969</v>
+        <v>270</v>
       </c>
       <c r="J32" t="n">
-        <v>175.8459615593269</v>
+        <v>276</v>
       </c>
       <c r="K32" t="n">
-        <v>176.3395177314362</v>
+        <v>155.5476692350085</v>
       </c>
       <c r="L32" t="n">
-        <v>180.7498642476663</v>
+        <v>160.1605965196842</v>
       </c>
       <c r="M32" t="b">
         <v>0</v>
@@ -2096,16 +2096,16 @@
         </is>
       </c>
       <c r="I33" t="n">
-        <v>180.7498642476662</v>
+        <v>282</v>
       </c>
       <c r="J33" t="n">
-        <v>192.1478497810181</v>
+        <v>300</v>
       </c>
       <c r="K33" t="n">
-        <v>180.7498642476663</v>
+        <v>160.1605965196842</v>
       </c>
       <c r="L33" t="n">
-        <v>192.1478497810181</v>
+        <v>172.3199422514753</v>
       </c>
       <c r="M33" t="b">
         <v>0</v>
@@ -2147,16 +2147,16 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>180.7498642476662</v>
+        <v>282</v>
       </c>
       <c r="J34" t="n">
-        <v>189.2052191264531</v>
+        <v>294</v>
       </c>
       <c r="K34" t="n">
-        <v>183.6924949022312</v>
+        <v>163.6395068759155</v>
       </c>
       <c r="L34" t="n">
-        <v>192.1478497810181</v>
+        <v>172.3199422514753</v>
       </c>
       <c r="M34" t="b">
         <v>0</v>
@@ -2198,16 +2198,16 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>180.7498642476662</v>
+        <v>282</v>
       </c>
       <c r="J35" t="n">
-        <v>185.5136351355464</v>
+        <v>288</v>
       </c>
       <c r="K35" t="n">
-        <v>187.3840788931379</v>
+        <v>167.9939303676939</v>
       </c>
       <c r="L35" t="n">
-        <v>192.1478497810181</v>
+        <v>172.3199422514753</v>
       </c>
       <c r="M35" t="b">
         <v>0</v>
@@ -2249,16 +2249,16 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>228.8551367811691</v>
+        <v>348</v>
       </c>
       <c r="J36" t="n">
-        <v>243.4515303145227</v>
+        <v>375</v>
       </c>
       <c r="K36" t="n">
-        <v>228.8551367811691</v>
+        <v>206.6224847608567</v>
       </c>
       <c r="L36" t="n">
-        <v>243.4515303145228</v>
+        <v>226.444825318454</v>
       </c>
       <c r="M36" t="b">
         <v>0</v>
@@ -2300,16 +2300,16 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>192.1478497810181</v>
+        <v>300</v>
       </c>
       <c r="J37" t="n">
-        <v>228.8551367811691</v>
+        <v>348</v>
       </c>
       <c r="K37" t="n">
-        <v>192.1478497810181</v>
+        <v>172.3199422514753</v>
       </c>
       <c r="L37" t="n">
-        <v>228.8551367811691</v>
+        <v>206.6224847608567</v>
       </c>
       <c r="M37" t="b">
         <v>0</v>
@@ -2351,16 +2351,16 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>192.1478497810181</v>
+        <v>300</v>
       </c>
       <c r="J38" t="n">
-        <v>220.4522987240683</v>
+        <v>342</v>
       </c>
       <c r="K38" t="n">
-        <v>200.5506878381189</v>
+        <v>185.8638278138747</v>
       </c>
       <c r="L38" t="n">
-        <v>228.8551367811691</v>
+        <v>206.6224847608567</v>
       </c>
       <c r="M38" t="b">
         <v>0</v>
@@ -2402,19 +2402,19 @@
         </is>
       </c>
       <c r="I39" t="n">
-        <v>243.4515303145227</v>
+        <v>375</v>
       </c>
       <c r="J39" t="n">
-        <v>264.7004036901122</v>
+        <v>402</v>
       </c>
       <c r="K39" t="n">
-        <v>243.4515303145228</v>
+        <v>226.444825318454</v>
       </c>
       <c r="L39" t="n">
-        <v>264.7004036901122</v>
+        <v>244.7998551128945</v>
       </c>
       <c r="M39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -2453,19 +2453,19 @@
         </is>
       </c>
       <c r="I40" t="n">
-        <v>264.7004036901122</v>
+        <v>402</v>
       </c>
       <c r="J40" t="n">
-        <v>290.3144387401048</v>
+        <v>444</v>
       </c>
       <c r="K40" t="n">
-        <v>264.7004036901122</v>
+        <v>244.7998551128945</v>
       </c>
       <c r="L40" t="n">
-        <v>290.3144387401048</v>
+        <v>270.7601128539436</v>
       </c>
       <c r="M40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -2504,16 +2504,16 @@
         </is>
       </c>
       <c r="I41" t="n">
-        <v>264.7004036901122</v>
+        <v>402</v>
       </c>
       <c r="J41" t="n">
-        <v>280.7060107955276</v>
+        <v>426</v>
       </c>
       <c r="K41" t="n">
-        <v>274.3088316346894</v>
+        <v>256.2211522002381</v>
       </c>
       <c r="L41" t="n">
-        <v>290.3144387401048</v>
+        <v>270.7601128539436</v>
       </c>
       <c r="M41" t="b">
         <v>0</v>
@@ -2555,16 +2555,16 @@
         </is>
       </c>
       <c r="I42" t="n">
-        <v>264.7004036901122</v>
+        <v>402</v>
       </c>
       <c r="J42" t="n">
-        <v>272.8739389404219</v>
+        <v>414</v>
       </c>
       <c r="K42" t="n">
-        <v>282.1409034897952</v>
+        <v>261.5344267486111</v>
       </c>
       <c r="L42" t="n">
-        <v>290.3144387401048</v>
+        <v>270.7601128539436</v>
       </c>
       <c r="M42" t="b">
         <v>0</v>
@@ -2606,16 +2606,16 @@
         </is>
       </c>
       <c r="I43" t="n">
-        <v>264.7004036901122</v>
+        <v>402</v>
       </c>
       <c r="J43" t="n">
-        <v>268.9095785547743</v>
+        <v>408</v>
       </c>
       <c r="K43" t="n">
-        <v>286.1052638754427</v>
+        <v>266.3181084792336</v>
       </c>
       <c r="L43" t="n">
-        <v>290.3144387401048</v>
+        <v>270.7601128539436</v>
       </c>
       <c r="M43" t="b">
         <v>0</v>
@@ -2657,16 +2657,16 @@
         </is>
       </c>
       <c r="I44" t="n">
-        <v>264.7004036901122</v>
+        <v>402</v>
       </c>
       <c r="J44" t="n">
-        <v>268.1740676862505</v>
+        <v>408</v>
       </c>
       <c r="K44" t="n">
-        <v>286.8407747439665</v>
+        <v>267.7386336360777</v>
       </c>
       <c r="L44" t="n">
-        <v>290.3144387401048</v>
+        <v>270.7601128539436</v>
       </c>
       <c r="M44" t="b">
         <v>0</v>
@@ -2708,16 +2708,16 @@
         </is>
       </c>
       <c r="I45" t="n">
-        <v>264.7004036901122</v>
+        <v>402</v>
       </c>
       <c r="J45" t="n">
-        <v>282.0679227718445</v>
+        <v>426</v>
       </c>
       <c r="K45" t="n">
-        <v>272.9469196583725</v>
+        <v>257.8184581014112</v>
       </c>
       <c r="L45" t="n">
-        <v>290.3144387401048</v>
+        <v>270.7601128539436</v>
       </c>
       <c r="M45" t="b">
         <v>0</v>
@@ -2759,16 +2759,16 @@
         </is>
       </c>
       <c r="I46" t="n">
-        <v>264.7004036901122</v>
+        <v>402</v>
       </c>
       <c r="J46" t="n">
-        <v>286.6332266547332</v>
+        <v>438</v>
       </c>
       <c r="K46" t="n">
-        <v>268.3816157754839</v>
+        <v>256.7869898520808</v>
       </c>
       <c r="L46" t="n">
-        <v>290.3144387401048</v>
+        <v>270.7601128539436</v>
       </c>
       <c r="M46" t="b">
         <v>0</v>
@@ -2810,19 +2810,19 @@
         </is>
       </c>
       <c r="I47" t="n">
-        <v>290.3144387401048</v>
+        <v>444</v>
       </c>
       <c r="J47" t="n">
-        <v>294.985074221542</v>
+        <v>453</v>
       </c>
       <c r="K47" t="n">
-        <v>290.3144387401048</v>
+        <v>270.7601128539436</v>
       </c>
       <c r="L47" t="n">
-        <v>294.985074221542</v>
+        <v>276.8332256961308</v>
       </c>
       <c r="M47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -2861,19 +2861,19 @@
         </is>
       </c>
       <c r="I48" t="n">
-        <v>294.985074221542</v>
+        <v>453</v>
       </c>
       <c r="J48" t="n">
-        <v>306.0306463389053</v>
+        <v>471</v>
       </c>
       <c r="K48" t="n">
-        <v>294.985074221542</v>
+        <v>276.8332256961308</v>
       </c>
       <c r="L48" t="n">
-        <v>306.0306463389053</v>
+        <v>290.5902879800396</v>
       </c>
       <c r="M48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -2912,16 +2912,16 @@
         </is>
       </c>
       <c r="I49" t="n">
-        <v>294.985074221542</v>
+        <v>453</v>
       </c>
       <c r="J49" t="n">
-        <v>303.3347119835435</v>
+        <v>465</v>
       </c>
       <c r="K49" t="n">
-        <v>297.6810085769039</v>
+        <v>282.1390808289829</v>
       </c>
       <c r="L49" t="n">
-        <v>306.0306463389053</v>
+        <v>290.5902879800396</v>
       </c>
       <c r="M49" t="b">
         <v>0</v>
@@ -2963,16 +2963,16 @@
         </is>
       </c>
       <c r="I50" t="n">
-        <v>294.985074221542</v>
+        <v>453</v>
       </c>
       <c r="J50" t="n">
-        <v>302.0891173277271</v>
+        <v>462</v>
       </c>
       <c r="K50" t="n">
-        <v>298.9266032327202</v>
+        <v>284.1284706169079</v>
       </c>
       <c r="L50" t="n">
-        <v>306.0306463389053</v>
+        <v>290.5902879800396</v>
       </c>
       <c r="M50" t="b">
         <v>0</v>
@@ -3014,19 +3014,19 @@
         </is>
       </c>
       <c r="I51" t="n">
-        <v>306.0306463389053</v>
+        <v>471</v>
       </c>
       <c r="J51" t="n">
-        <v>312.5289269206861</v>
+        <v>483</v>
       </c>
       <c r="K51" t="n">
-        <v>306.0306463389053</v>
+        <v>290.5902879800396</v>
       </c>
       <c r="L51" t="n">
-        <v>312.5289269206861</v>
+        <v>299.0420988685125</v>
       </c>
       <c r="M51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -3065,19 +3065,19 @@
         </is>
       </c>
       <c r="I52" t="n">
-        <v>312.5289269206861</v>
+        <v>483</v>
       </c>
       <c r="J52" t="n">
-        <v>328.2473415385353</v>
+        <v>510</v>
       </c>
       <c r="K52" t="n">
-        <v>312.5289269206861</v>
+        <v>299.0420988685125</v>
       </c>
       <c r="L52" t="n">
-        <v>328.2473415385353</v>
+        <v>315.9740768080833</v>
       </c>
       <c r="M52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -3116,16 +3116,16 @@
         </is>
       </c>
       <c r="I53" t="n">
-        <v>328.2473415385353</v>
+        <v>510</v>
       </c>
       <c r="J53" t="n">
-        <v>332.8794222485922</v>
+        <v>516</v>
       </c>
       <c r="K53" t="n">
-        <v>331.9554020630753</v>
+        <v>324.5192611168119</v>
       </c>
       <c r="L53" t="n">
-        <v>336.5874827731322</v>
+        <v>329.2830629108927</v>
       </c>
       <c r="M53" t="b">
         <v>0</v>
@@ -3167,19 +3167,19 @@
         </is>
       </c>
       <c r="I54" t="n">
-        <v>328.2473415385353</v>
+        <v>510</v>
       </c>
       <c r="J54" t="n">
-        <v>336.5874827731322</v>
+        <v>528</v>
       </c>
       <c r="K54" t="n">
-        <v>328.2473415385353</v>
+        <v>315.9740768080833</v>
       </c>
       <c r="L54" t="n">
-        <v>336.5874827731322</v>
+        <v>329.2830629108927</v>
       </c>
       <c r="M54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -3218,16 +3218,16 @@
         </is>
       </c>
       <c r="I55" t="n">
-        <v>328.2473415385353</v>
+        <v>510</v>
       </c>
       <c r="J55" t="n">
-        <v>332.1083260848313</v>
+        <v>516</v>
       </c>
       <c r="K55" t="n">
-        <v>332.7264982268362</v>
+        <v>325.2030717683239</v>
       </c>
       <c r="L55" t="n">
-        <v>336.5874827731322</v>
+        <v>329.2830629108927</v>
       </c>
       <c r="M55" t="b">
         <v>0</v>
@@ -3269,16 +3269,16 @@
         </is>
       </c>
       <c r="I56" t="n">
-        <v>336.5874827731322</v>
+        <v>528</v>
       </c>
       <c r="J56" t="n">
-        <v>339.7332721767947</v>
+        <v>534</v>
       </c>
       <c r="K56" t="n">
-        <v>337.995023081273</v>
+        <v>329.5299216078971</v>
       </c>
       <c r="L56" t="n">
-        <v>341.1408124849355</v>
+        <v>333.4440938846141</v>
       </c>
       <c r="M56" t="b">
         <v>0</v>
@@ -3320,19 +3320,19 @@
         </is>
       </c>
       <c r="I57" t="n">
-        <v>336.5874827731322</v>
+        <v>528</v>
       </c>
       <c r="J57" t="n">
-        <v>341.1408124849355</v>
+        <v>534</v>
       </c>
       <c r="K57" t="n">
-        <v>336.5874827731322</v>
+        <v>329.2830629108927</v>
       </c>
       <c r="L57" t="n">
-        <v>341.1408124849355</v>
+        <v>333.4440938846141</v>
       </c>
       <c r="M57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -3371,16 +3371,16 @@
         </is>
       </c>
       <c r="I58" t="n">
-        <v>341.1408124849355</v>
+        <v>534</v>
       </c>
       <c r="J58" t="n">
-        <v>344.7884643605551</v>
+        <v>540</v>
       </c>
       <c r="K58" t="n">
-        <v>342.1062684793792</v>
+        <v>336.0659134034996</v>
       </c>
       <c r="L58" t="n">
-        <v>345.7539203549987</v>
+        <v>340.3465076658096</v>
       </c>
       <c r="M58" t="b">
         <v>0</v>
@@ -3422,19 +3422,19 @@
         </is>
       </c>
       <c r="I59" t="n">
-        <v>341.1408124849355</v>
+        <v>534</v>
       </c>
       <c r="J59" t="n">
-        <v>345.7539203549987</v>
+        <v>543</v>
       </c>
       <c r="K59" t="n">
-        <v>341.1408124849355</v>
+        <v>333.4440938846141</v>
       </c>
       <c r="L59" t="n">
-        <v>345.7539203549987</v>
+        <v>340.3465076658096</v>
       </c>
       <c r="M59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -3473,16 +3473,16 @@
         </is>
       </c>
       <c r="I60" t="n">
-        <v>341.1408124849355</v>
+        <v>534</v>
       </c>
       <c r="J60" t="n">
-        <v>344.876812688411</v>
+        <v>540</v>
       </c>
       <c r="K60" t="n">
-        <v>342.0179201515233</v>
+        <v>336.8593551736687</v>
       </c>
       <c r="L60" t="n">
-        <v>345.7539203549987</v>
+        <v>340.3465076658096</v>
       </c>
       <c r="M60" t="b">
         <v>0</v>
@@ -3524,19 +3524,19 @@
         </is>
       </c>
       <c r="I61" t="n">
-        <v>345.7539203549987</v>
+        <v>543</v>
       </c>
       <c r="J61" t="n">
-        <v>349.3209873849102</v>
+        <v>549</v>
       </c>
       <c r="K61" t="n">
-        <v>345.7539203549987</v>
+        <v>340.3465076658096</v>
       </c>
       <c r="L61" t="n">
-        <v>349.3209873849102</v>
+        <v>345.0811463029151</v>
       </c>
       <c r="M61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -3575,19 +3575,19 @@
         </is>
       </c>
       <c r="I62" t="n">
-        <v>349.3209873849102</v>
+        <v>549</v>
       </c>
       <c r="J62" t="n">
-        <v>353.1484317802756</v>
+        <v>555</v>
       </c>
       <c r="K62" t="n">
-        <v>349.3209873849102</v>
+        <v>345.0811463029151</v>
       </c>
       <c r="L62" t="n">
-        <v>353.1484317802756</v>
+        <v>349.2397617328445</v>
       </c>
       <c r="M62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -3626,19 +3626,19 @@
         </is>
       </c>
       <c r="I63" t="n">
-        <v>353.1484317802756</v>
+        <v>555</v>
       </c>
       <c r="J63" t="n">
-        <v>354.1484317802756</v>
+        <v>556</v>
       </c>
       <c r="K63" t="n">
-        <v>353.1484317802756</v>
+        <v>349.2397617328445</v>
       </c>
       <c r="L63" t="n">
-        <v>354.1484317802756</v>
+        <v>350.2397617328445</v>
       </c>
       <c r="M63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -3668,19 +3668,19 @@
       </c>
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="n">
-        <v>354.1484317802756</v>
+        <v>556</v>
       </c>
       <c r="J64" t="n">
-        <v>354.1484317802756</v>
+        <v>556</v>
       </c>
       <c r="K64" t="n">
-        <v>354.1484317802756</v>
+        <v>350.2397617328445</v>
       </c>
       <c r="L64" t="n">
-        <v>354.1484317802756</v>
+        <v>350.2397617328445</v>
       </c>
       <c r="M64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>